<commit_message>
s Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/tablas excel (version 1).xlsx
+++ b/tablas excel (version 1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex0\Documents\CEU\bases de datos\BaseDatosRestaurante\BasesDatosRestaurante\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Escritorio\CEU San Pablo\20-21\Segundo Cuatrimestre\Tratamiento de la Información en Sistemas Distribuidos\Workspace\BasesDatosRestaurante\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A69327-A900-4BE4-8581-98E856B7C50B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22948564-1CCB-41ED-A711-B0D16B8F4FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A57DBF19-0EB8-477C-8A9B-FEE33F6BE215}"/>
   </bookViews>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>Pedidos</t>
   </si>
@@ -54,12 +53,6 @@
     <t>Cargo-id</t>
   </si>
   <si>
-    <t>Jefe-id</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
     <t>Clientes</t>
   </si>
   <si>
@@ -69,9 +62,6 @@
     <t>Jefes</t>
   </si>
   <si>
-    <t>Miguel</t>
-  </si>
-  <si>
     <t>Cargo</t>
   </si>
   <si>
@@ -99,18 +89,12 @@
     <t>Dir.entrega</t>
   </si>
   <si>
-    <t>43$</t>
-  </si>
-  <si>
     <t>Av.juan rallo 16</t>
   </si>
   <si>
     <t>Empleados</t>
   </si>
   <si>
-    <t>id-emple</t>
-  </si>
-  <si>
     <t>id-pedido</t>
   </si>
   <si>
@@ -129,9 +113,6 @@
     <t>precio</t>
   </si>
   <si>
-    <t>patatas</t>
-  </si>
-  <si>
     <t>3$</t>
   </si>
   <si>
@@ -144,19 +125,130 @@
     <t>id-menu</t>
   </si>
   <si>
-    <t>id-cliente</t>
-  </si>
-  <si>
-    <t>cliente-pedidos</t>
-  </si>
-  <si>
-    <t>empleado(repartidor)-pedidos</t>
-  </si>
-  <si>
-    <t>pedidos-menus</t>
-  </si>
-  <si>
-    <t>1300$</t>
+    <t>Croquetas</t>
+  </si>
+  <si>
+    <t>Fingers Pollo</t>
+  </si>
+  <si>
+    <t>Calamares</t>
+  </si>
+  <si>
+    <t>7$</t>
+  </si>
+  <si>
+    <t>Pulpo a la gallega</t>
+  </si>
+  <si>
+    <t>15$</t>
+  </si>
+  <si>
+    <t>Plato de Pasta</t>
+  </si>
+  <si>
+    <t>Escalope</t>
+  </si>
+  <si>
+    <t>Cahopo</t>
+  </si>
+  <si>
+    <t>Chuleton de Buey</t>
+  </si>
+  <si>
+    <t>25$</t>
+  </si>
+  <si>
+    <t>patatas 4 salsas</t>
+  </si>
+  <si>
+    <t>20$</t>
+  </si>
+  <si>
+    <t>6$</t>
+  </si>
+  <si>
+    <t>14$</t>
+  </si>
+  <si>
+    <t>12$</t>
+  </si>
+  <si>
+    <t>16$</t>
+  </si>
+  <si>
+    <t>Solomillo</t>
+  </si>
+  <si>
+    <t>30$</t>
+  </si>
+  <si>
+    <t>Informatico</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>1200$</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>1400$</t>
+  </si>
+  <si>
+    <t>1100$</t>
+  </si>
+  <si>
+    <t>Marta</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Enriqueta</t>
+  </si>
+  <si>
+    <t>Alfredo</t>
+  </si>
+  <si>
+    <t>Eusebio</t>
+  </si>
+  <si>
+    <t>Valentin</t>
+  </si>
+  <si>
+    <t>Pedido - Repartidor</t>
+  </si>
+  <si>
+    <t>Pedido-Menu</t>
+  </si>
+  <si>
+    <t>27$</t>
+  </si>
+  <si>
+    <t>id-Empleado</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Jordan@gmail.com</t>
+  </si>
+  <si>
+    <t>33$</t>
+  </si>
+  <si>
+    <t>Calle Pepito 12</t>
   </si>
 </sst>
 </file>
@@ -196,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -208,19 +300,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -263,16 +342,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -591,23 +669,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3914556A-80B6-47D8-98B9-EA7C1BB7DC75}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="6" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,314 +695,599 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2" s="10"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>4</v>
-      </c>
-      <c r="C3" s="10">
+        <v>14</v>
+      </c>
+      <c r="C3" s="9">
         <v>44481</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4">
         <v>0.89583333333333337</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9">
+        <v>44278</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="6"/>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>653213498</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2</v>
+      </c>
+      <c r="J22" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2">
+        <v>675432651</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>4</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="B39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="B40" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C40" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="B41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>8</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J10" s="1" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>9</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>10</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2">
-        <v>653213498</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="C44" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>11</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="2">
-        <v>3</v>
-      </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E22" s="2">
-        <v>7</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>4</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="11"/>
+      <c r="C45" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" xr:uid="{3FE0FA66-4998-40D9-B876-62145EC6BCDB}"/>
+    <hyperlink ref="D22" r:id="rId1" xr:uid="{3FE0FA66-4998-40D9-B876-62145EC6BCDB}"/>
+    <hyperlink ref="D23" r:id="rId2" xr:uid="{B2291824-1A8C-48F3-ABA3-B8E6A450EE7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>